<commit_message>
updating files and uploading presentation
</commit_message>
<xml_diff>
--- a/Prophet/Business Analysis.xlsx
+++ b/Prophet/Business Analysis.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esdras/Ironhack/Proyect/Prophet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{02AC5E22-E0AD-494E-85A2-F5ECABD98CAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8F9B07-AE40-4F4D-8421-8BD83C33E4AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="27560" windowHeight="17040"/>
+    <workbookView xWindow="880" yWindow="460" windowWidth="27560" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final" sheetId="1" r:id="rId1"/>
@@ -95,9 +95,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Cost P/H</t>
-  </si>
-  <si>
     <t>Regular</t>
   </si>
   <si>
@@ -120,17 +117,20 @@
   </si>
   <si>
     <t>Perid savings</t>
+  </si>
+  <si>
+    <t>Cost P/D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -455,7 +455,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -570,6 +570,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -618,16 +644,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -636,14 +662,25 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="22" builtinId="30" customBuiltin="1"/>
@@ -1001,11 +1038,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="M6" sqref="M6:S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1017,10 +1054,11 @@
     <col min="9" max="9" width="2.1640625" customWidth="1"/>
     <col min="10" max="11" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.1640625" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1221,8 +1259,8 @@
         <f t="shared" si="3"/>
         <v>0.89940266448915829</v>
       </c>
-      <c r="M6" t="s">
-        <v>26</v>
+      <c r="M6" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
@@ -1258,16 +1296,16 @@
         <f t="shared" si="3"/>
         <v>0.1652295502213936</v>
       </c>
-      <c r="P7" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q7" t="s">
+      <c r="P7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="R7" t="s">
+      <c r="Q7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="R7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="S7" t="s">
+      <c r="S7" s="9" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1304,22 +1342,22 @@
         <f t="shared" si="3"/>
         <v>-1</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="N8" t="s">
-        <v>24</v>
-      </c>
-      <c r="O8" t="s">
-        <v>21</v>
-      </c>
-      <c r="P8" s="1">
+      <c r="N8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="P8" s="19">
         <v>11363</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="Q8" s="19">
         <v>9090</v>
       </c>
-      <c r="R8" s="1">
+      <c r="R8" s="19">
         <v>7727</v>
       </c>
     </row>
@@ -1356,7 +1394,7 @@
         <f t="shared" si="3"/>
         <v>-0.2447050678191908</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="4">
         <v>4</v>
       </c>
       <c r="N9" t="s">
@@ -1365,13 +1403,13 @@
       <c r="O9" t="s">
         <v>11</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="4">
         <v>1</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="4">
         <v>1</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="4">
         <v>2</v>
       </c>
       <c r="S9" s="13">
@@ -1412,22 +1450,22 @@
         <f t="shared" si="3"/>
         <v>-0.57881095091527623</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="4">
         <v>8</v>
       </c>
       <c r="N10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O10" t="s">
         <v>12</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="4">
         <v>2</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="4">
         <v>3</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="4">
         <v>3</v>
       </c>
       <c r="S10" s="13">
@@ -1445,7 +1483,7 @@
       <c r="C11" s="1">
         <v>274174</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="15">
         <v>250875.64301471101</v>
       </c>
       <c r="E11" s="11">
@@ -1468,7 +1506,7 @@
         <f t="shared" si="3"/>
         <v>-6.9933691743199577E-2</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="4">
         <v>7</v>
       </c>
       <c r="N11" t="s">
@@ -1477,13 +1515,13 @@
       <c r="O11" t="s">
         <v>13</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="4">
         <v>1</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="4">
         <v>4</v>
       </c>
-      <c r="R11">
+      <c r="R11" s="4">
         <v>2</v>
       </c>
       <c r="S11" s="13">
@@ -1524,7 +1562,7 @@
         <f t="shared" si="3"/>
         <v>0.51227706364694214</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="4">
         <v>5</v>
       </c>
       <c r="N12" s="12" t="s">
@@ -1533,13 +1571,13 @@
       <c r="O12" t="s">
         <v>14</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="4">
         <v>1</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="4">
         <v>2</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="4">
         <v>2</v>
       </c>
       <c r="S12" s="13">
@@ -1580,7 +1618,7 @@
         <f t="shared" si="3"/>
         <v>0.77011910982202836</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="4">
         <v>3</v>
       </c>
       <c r="N13" t="s">
@@ -1589,10 +1627,11 @@
       <c r="O13" t="s">
         <v>15</v>
       </c>
-      <c r="Q13">
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4">
         <v>2</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="4">
         <v>1</v>
       </c>
       <c r="S13" s="13">
@@ -1600,7 +1639,7 @@
         <v>25907</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>546</v>
       </c>
@@ -1633,7 +1672,10 @@
         <f t="shared" si="3"/>
         <v>-1</v>
       </c>
-      <c r="S14" s="15">
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="17">
         <f>SUM(S9:S13)</f>
         <v>243165</v>
       </c>
@@ -1671,6 +1713,9 @@
         <f t="shared" si="3"/>
         <v>-0.27786406038243527</v>
       </c>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -1705,11 +1750,14 @@
         <f t="shared" si="3"/>
         <v>-0.41906005221932113</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M16" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>549</v>
       </c>
@@ -1742,20 +1790,24 @@
         <f t="shared" si="3"/>
         <v>-2.7473863360077802E-2</v>
       </c>
-      <c r="P17" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q17" t="s">
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="R17" t="s">
+      <c r="Q17" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="R17" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="S17" t="s">
+      <c r="S17" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="W17" s="4"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>550</v>
       </c>
@@ -1788,26 +1840,26 @@
         <f t="shared" si="3"/>
         <v>0.22085873048645835</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M18" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="N18" t="s">
-        <v>24</v>
-      </c>
-      <c r="O18" t="s">
-        <v>21</v>
-      </c>
-      <c r="P18" s="1">
+      <c r="N18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="O18" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="P18" s="20">
         <v>11363</v>
       </c>
-      <c r="Q18" s="1">
+      <c r="Q18" s="20">
         <v>9090</v>
       </c>
-      <c r="R18" s="1">
+      <c r="R18" s="20">
         <v>7727</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>551</v>
       </c>
@@ -1840,7 +1892,7 @@
         <f t="shared" si="3"/>
         <v>-7.3195235133712861E-3</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="4">
         <v>4</v>
       </c>
       <c r="N19" t="s">
@@ -1849,13 +1901,13 @@
       <c r="O19" t="s">
         <v>11</v>
       </c>
-      <c r="P19">
+      <c r="P19" s="4">
         <v>1</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="4">
         <v>1</v>
       </c>
-      <c r="R19">
+      <c r="R19" s="4">
         <v>2</v>
       </c>
       <c r="S19" s="13">
@@ -1863,7 +1915,7 @@
         <v>35907</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>552</v>
       </c>
@@ -1896,22 +1948,22 @@
         <f t="shared" si="3"/>
         <v>-1</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="21">
         <v>7</v>
       </c>
       <c r="N20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O20" t="s">
         <v>12</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="4">
         <v>1</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" s="4">
         <v>3</v>
       </c>
-      <c r="R20">
+      <c r="R20" s="4">
         <v>3</v>
       </c>
       <c r="S20" s="13">
@@ -1919,7 +1971,7 @@
         <v>61814</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>553</v>
       </c>
@@ -1952,7 +2004,7 @@
         <f t="shared" si="3"/>
         <v>-0.31110620446014575</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="4">
         <v>7</v>
       </c>
       <c r="N21" t="s">
@@ -1961,13 +2013,13 @@
       <c r="O21" t="s">
         <v>13</v>
       </c>
-      <c r="P21">
+      <c r="P21" s="4">
         <v>1</v>
       </c>
-      <c r="Q21">
+      <c r="Q21" s="4">
         <v>4</v>
       </c>
-      <c r="R21">
+      <c r="R21" s="4">
         <v>2</v>
       </c>
       <c r="S21" s="13">
@@ -1975,7 +2027,7 @@
         <v>63177</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>554</v>
       </c>
@@ -2008,7 +2060,7 @@
         <f t="shared" si="3"/>
         <v>-0.41512867169222772</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="4">
         <v>5</v>
       </c>
       <c r="N22" s="12" t="s">
@@ -2017,13 +2069,13 @@
       <c r="O22" t="s">
         <v>14</v>
       </c>
-      <c r="P22">
+      <c r="P22" s="4">
         <v>1</v>
       </c>
-      <c r="Q22">
+      <c r="Q22" s="4">
         <v>2</v>
       </c>
-      <c r="R22">
+      <c r="R22" s="4">
         <v>1</v>
       </c>
       <c r="S22" s="13">
@@ -2031,7 +2083,7 @@
         <v>37270</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>555</v>
       </c>
@@ -2064,7 +2116,7 @@
         <f t="shared" si="3"/>
         <v>-0.1029284269338214</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="21">
         <v>2.5</v>
       </c>
       <c r="N23" t="s">
@@ -2073,10 +2125,11 @@
       <c r="O23" t="s">
         <v>15</v>
       </c>
-      <c r="Q23">
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4">
         <v>2</v>
       </c>
-      <c r="R23">
+      <c r="R23" s="4">
         <v>0.5</v>
       </c>
       <c r="S23" s="13">
@@ -2084,7 +2137,7 @@
         <v>22043.5</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>556</v>
       </c>
@@ -2117,12 +2170,15 @@
         <f t="shared" si="3"/>
         <v>0.71606234353549225</v>
       </c>
-      <c r="S24" s="15">
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="17">
         <f>SUM(S19:S23)</f>
         <v>220211.5</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>557</v>
       </c>
@@ -2156,7 +2212,7 @@
         <v>7.2205373280642096E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>558</v>
       </c>
@@ -2190,7 +2246,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>559</v>
       </c>
@@ -2223,15 +2279,16 @@
         <f t="shared" si="3"/>
         <v>-0.25376798075506896</v>
       </c>
-      <c r="R27" t="s">
-        <v>29</v>
-      </c>
+      <c r="Q27" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="R27" s="18"/>
       <c r="S27" s="14">
         <f>S14-S24</f>
         <v>22953.5</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C28" s="6">
         <f>SUM(C2:C27)</f>
         <v>3968066</v>
@@ -2246,35 +2303,37 @@
         <f>SUM(G2:G27)</f>
         <v>3606000</v>
       </c>
-      <c r="R28" t="s">
-        <v>27</v>
-      </c>
-      <c r="S28" s="17">
+      <c r="Q28" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="R28" s="18"/>
+      <c r="S28" s="14">
         <f>S27*3</f>
         <v>68860.5</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="E29" s="2"/>
       <c r="H29" s="2"/>
       <c r="J29" s="3"/>
-      <c r="R29" t="s">
-        <v>28</v>
-      </c>
-      <c r="S29" s="17">
+      <c r="Q29" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="R29" s="18"/>
+      <c r="S29" s="14">
         <f>S28*12</f>
         <v>826326</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>5</v>
       </c>
@@ -2303,6 +2362,11 @@
       <c r="F33" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="Q29:R29"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>